<commit_message>
New version of the distributed model
</commit_message>
<xml_diff>
--- a/2_MegaWat/3_PointScale_version/3_Inputs/2_Apennine/Parameters_TC.xlsx
+++ b/2_MegaWat/3_PointScale_version/3_Inputs/2_Apennine/Parameters_TC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrodrigu\Desktop\19_ISTA\1_TC\3_Model_Source\2_MegaWat\3_PointScale_version\3_Inputs\2_Apennine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrodrigu\Desktop\19_ISTA\1_Science_MegaWat\1_TC\3_Model_Source\2_MegaWat\3_PointScale_version\3_Inputs\2_Apennine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F75FE2-3D85-44E8-BD5A-4FD575B42F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ABE0B7-7F64-42A6-AFFF-D59E7B9D5FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -215,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="315">
   <si>
     <t>Crops_WW</t>
   </si>
@@ -1157,6 +1160,9 @@
   </si>
   <si>
     <t>EvGreen_NeedLeaves_LeBray</t>
+  </si>
+  <si>
+    <t>No/Max</t>
   </si>
 </sst>
 </file>
@@ -1206,7 +1212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1231,6 +1237,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1244,7 +1256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1327,6 +1339,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1646,10 +1661,10 @@
   <dimension ref="A1:AK188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD13" sqref="AD13"/>
+      <selection pane="bottomRight" activeCell="AF171" sqref="AF171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14851,7 +14866,7 @@
         <v>151</v>
       </c>
       <c r="D137" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E137" s="19"/>
       <c r="F137" s="19"/>
@@ -14870,65 +14885,65 @@
       <c r="K137" s="21">
         <v>0</v>
       </c>
-      <c r="L137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W137" s="21" t="s">
-        <v>14</v>
+      <c r="L137" s="30">
+        <v>0</v>
+      </c>
+      <c r="M137" s="30">
+        <v>0</v>
+      </c>
+      <c r="N137" s="30">
+        <v>0</v>
+      </c>
+      <c r="O137" s="30">
+        <v>0</v>
+      </c>
+      <c r="P137" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="30">
+        <v>0</v>
+      </c>
+      <c r="R137" s="30">
+        <v>0</v>
+      </c>
+      <c r="S137" s="30">
+        <v>0</v>
+      </c>
+      <c r="T137" s="30">
+        <v>0</v>
+      </c>
+      <c r="U137" s="30">
+        <v>0</v>
+      </c>
+      <c r="V137" s="30">
+        <v>0</v>
+      </c>
+      <c r="W137" s="30">
+        <v>0</v>
       </c>
       <c r="X137" s="21">
         <v>368.55</v>
       </c>
-      <c r="Y137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD137" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE137" s="21" t="s">
-        <v>14</v>
+      <c r="Y137" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z137" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA137" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB137" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC137" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD137" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE137" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:31" x14ac:dyDescent="0.35">
@@ -14942,7 +14957,7 @@
         <v>151</v>
       </c>
       <c r="D138" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E138" s="19"/>
       <c r="F138" s="19"/>
@@ -14961,65 +14976,65 @@
       <c r="K138" s="21">
         <v>368.55</v>
       </c>
-      <c r="L138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W138" s="21" t="s">
-        <v>14</v>
+      <c r="L138" s="30">
+        <v>0</v>
+      </c>
+      <c r="M138" s="30">
+        <v>0</v>
+      </c>
+      <c r="N138" s="30">
+        <v>0</v>
+      </c>
+      <c r="O138" s="30">
+        <v>0</v>
+      </c>
+      <c r="P138" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="30">
+        <v>0</v>
+      </c>
+      <c r="R138" s="30">
+        <v>0</v>
+      </c>
+      <c r="S138" s="30">
+        <v>0</v>
+      </c>
+      <c r="T138" s="30">
+        <v>0</v>
+      </c>
+      <c r="U138" s="30">
+        <v>0</v>
+      </c>
+      <c r="V138" s="30">
+        <v>0</v>
+      </c>
+      <c r="W138" s="30">
+        <v>0</v>
       </c>
       <c r="X138" s="21">
         <v>0</v>
       </c>
-      <c r="Y138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD138" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE138" s="21" t="s">
-        <v>14</v>
+      <c r="Y138" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z138" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA138" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB138" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC138" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD138" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE138" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:31" x14ac:dyDescent="0.35">
@@ -15033,7 +15048,7 @@
         <v>151</v>
       </c>
       <c r="D139" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E139" s="19"/>
       <c r="F139" s="19"/>
@@ -15052,65 +15067,65 @@
       <c r="K139" s="21">
         <v>0</v>
       </c>
-      <c r="L139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W139" s="21" t="s">
-        <v>14</v>
+      <c r="L139" s="30">
+        <v>0</v>
+      </c>
+      <c r="M139" s="30">
+        <v>0</v>
+      </c>
+      <c r="N139" s="30">
+        <v>0</v>
+      </c>
+      <c r="O139" s="30">
+        <v>0</v>
+      </c>
+      <c r="P139" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="30">
+        <v>0</v>
+      </c>
+      <c r="R139" s="30">
+        <v>0</v>
+      </c>
+      <c r="S139" s="30">
+        <v>0</v>
+      </c>
+      <c r="T139" s="30">
+        <v>0</v>
+      </c>
+      <c r="U139" s="30">
+        <v>0</v>
+      </c>
+      <c r="V139" s="30">
+        <v>0</v>
+      </c>
+      <c r="W139" s="30">
+        <v>0</v>
       </c>
       <c r="X139" s="21">
         <v>368.55</v>
       </c>
-      <c r="Y139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD139" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE139" s="21" t="s">
-        <v>14</v>
+      <c r="Y139" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z139" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA139" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB139" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC139" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD139" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE139" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:31" x14ac:dyDescent="0.35">
@@ -15124,7 +15139,7 @@
         <v>151</v>
       </c>
       <c r="D140" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E140" s="19"/>
       <c r="F140" s="19"/>
@@ -15143,65 +15158,65 @@
       <c r="K140" s="21">
         <v>368.55</v>
       </c>
-      <c r="L140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W140" s="21" t="s">
-        <v>14</v>
+      <c r="L140" s="30">
+        <v>0</v>
+      </c>
+      <c r="M140" s="30">
+        <v>0</v>
+      </c>
+      <c r="N140" s="30">
+        <v>0</v>
+      </c>
+      <c r="O140" s="30">
+        <v>0</v>
+      </c>
+      <c r="P140" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="30">
+        <v>0</v>
+      </c>
+      <c r="R140" s="30">
+        <v>0</v>
+      </c>
+      <c r="S140" s="30">
+        <v>0</v>
+      </c>
+      <c r="T140" s="30">
+        <v>0</v>
+      </c>
+      <c r="U140" s="30">
+        <v>0</v>
+      </c>
+      <c r="V140" s="30">
+        <v>0</v>
+      </c>
+      <c r="W140" s="30">
+        <v>0</v>
       </c>
       <c r="X140" s="21">
         <v>0</v>
       </c>
-      <c r="Y140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD140" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE140" s="21" t="s">
-        <v>14</v>
+      <c r="Y140" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z140" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA140" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB140" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC140" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD140" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE140" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:31" x14ac:dyDescent="0.35">
@@ -15579,7 +15594,7 @@
         <v>151</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E145" s="19"/>
       <c r="F145" s="19"/>
@@ -15598,65 +15613,65 @@
       <c r="K145" s="21">
         <v>0</v>
       </c>
-      <c r="L145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="X145" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD145" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE145" s="21" t="s">
-        <v>14</v>
+      <c r="L145" s="30">
+        <v>1</v>
+      </c>
+      <c r="M145" s="30">
+        <v>1</v>
+      </c>
+      <c r="N145" s="30">
+        <v>1</v>
+      </c>
+      <c r="O145" s="30">
+        <v>1</v>
+      </c>
+      <c r="P145" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q145" s="30">
+        <v>1</v>
+      </c>
+      <c r="R145" s="30">
+        <v>1</v>
+      </c>
+      <c r="S145" s="30">
+        <v>1</v>
+      </c>
+      <c r="T145" s="30">
+        <v>1</v>
+      </c>
+      <c r="U145" s="30">
+        <v>1</v>
+      </c>
+      <c r="V145" s="30">
+        <v>1</v>
+      </c>
+      <c r="W145" s="30">
+        <v>1</v>
+      </c>
+      <c r="X145" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y145" s="30">
+        <v>1</v>
+      </c>
+      <c r="Z145" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA145" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB145" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC145" s="30">
+        <v>1</v>
+      </c>
+      <c r="AD145" s="30">
+        <v>1</v>
+      </c>
+      <c r="AE145" s="30">
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:31" x14ac:dyDescent="0.35">
@@ -15670,7 +15685,7 @@
         <v>151</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E146" s="19"/>
       <c r="F146" s="19"/>
@@ -15689,65 +15704,65 @@
       <c r="K146" s="21">
         <v>1</v>
       </c>
-      <c r="L146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="X146" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD146" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE146" s="21" t="s">
-        <v>14</v>
+      <c r="L146" s="30">
+        <v>1</v>
+      </c>
+      <c r="M146" s="30">
+        <v>1</v>
+      </c>
+      <c r="N146" s="30">
+        <v>1</v>
+      </c>
+      <c r="O146" s="30">
+        <v>1</v>
+      </c>
+      <c r="P146" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q146" s="30">
+        <v>1</v>
+      </c>
+      <c r="R146" s="30">
+        <v>1</v>
+      </c>
+      <c r="S146" s="30">
+        <v>1</v>
+      </c>
+      <c r="T146" s="30">
+        <v>1</v>
+      </c>
+      <c r="U146" s="30">
+        <v>1</v>
+      </c>
+      <c r="V146" s="30">
+        <v>1</v>
+      </c>
+      <c r="W146" s="30">
+        <v>1</v>
+      </c>
+      <c r="X146" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y146" s="30">
+        <v>1</v>
+      </c>
+      <c r="Z146" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA146" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB146" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC146" s="30">
+        <v>1</v>
+      </c>
+      <c r="AD146" s="30">
+        <v>1</v>
+      </c>
+      <c r="AE146" s="30">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:31" x14ac:dyDescent="0.35">
@@ -17763,7 +17778,7 @@
         <v>151</v>
       </c>
       <c r="D169" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E169" s="19"/>
       <c r="F169" s="19"/>
@@ -17782,65 +17797,65 @@
       <c r="K169" s="21">
         <v>0</v>
       </c>
-      <c r="L169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W169" s="21" t="s">
-        <v>14</v>
+      <c r="L169" s="30">
+        <v>0</v>
+      </c>
+      <c r="M169" s="30">
+        <v>0</v>
+      </c>
+      <c r="N169" s="30">
+        <v>0</v>
+      </c>
+      <c r="O169" s="30">
+        <v>0</v>
+      </c>
+      <c r="P169" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q169" s="30">
+        <v>0</v>
+      </c>
+      <c r="R169" s="30">
+        <v>0</v>
+      </c>
+      <c r="S169" s="30">
+        <v>0</v>
+      </c>
+      <c r="T169" s="30">
+        <v>0</v>
+      </c>
+      <c r="U169" s="30">
+        <v>0</v>
+      </c>
+      <c r="V169" s="30">
+        <v>0</v>
+      </c>
+      <c r="W169" s="30">
+        <v>0</v>
       </c>
       <c r="X169" s="21">
         <v>0</v>
       </c>
-      <c r="Y169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD169" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE169" s="21" t="s">
-        <v>14</v>
+      <c r="Y169" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z169" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA169" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB169" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC169" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD169" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE169" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:31" x14ac:dyDescent="0.35">
@@ -17854,7 +17869,7 @@
         <v>151</v>
       </c>
       <c r="D170" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E170" s="19"/>
       <c r="F170" s="19"/>
@@ -17873,65 +17888,65 @@
       <c r="K170" s="21">
         <v>0</v>
       </c>
-      <c r="L170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W170" s="21" t="s">
-        <v>14</v>
+      <c r="L170" s="30">
+        <v>0</v>
+      </c>
+      <c r="M170" s="30">
+        <v>0</v>
+      </c>
+      <c r="N170" s="30">
+        <v>0</v>
+      </c>
+      <c r="O170" s="30">
+        <v>0</v>
+      </c>
+      <c r="P170" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q170" s="30">
+        <v>0</v>
+      </c>
+      <c r="R170" s="30">
+        <v>0</v>
+      </c>
+      <c r="S170" s="30">
+        <v>0</v>
+      </c>
+      <c r="T170" s="30">
+        <v>0</v>
+      </c>
+      <c r="U170" s="30">
+        <v>0</v>
+      </c>
+      <c r="V170" s="30">
+        <v>0</v>
+      </c>
+      <c r="W170" s="30">
+        <v>0</v>
       </c>
       <c r="X170" s="21">
         <v>0</v>
       </c>
-      <c r="Y170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD170" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE170" s="21" t="s">
-        <v>14</v>
+      <c r="Y170" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z170" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA170" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB170" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC170" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD170" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE170" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:31" x14ac:dyDescent="0.35">
@@ -17945,7 +17960,7 @@
         <v>151</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E171" s="19"/>
       <c r="F171" s="19"/>
@@ -17964,65 +17979,65 @@
       <c r="K171" s="21">
         <v>0</v>
       </c>
-      <c r="L171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W171" s="21" t="s">
-        <v>14</v>
+      <c r="L171" s="30">
+        <v>0</v>
+      </c>
+      <c r="M171" s="30">
+        <v>0</v>
+      </c>
+      <c r="N171" s="30">
+        <v>0</v>
+      </c>
+      <c r="O171" s="30">
+        <v>0</v>
+      </c>
+      <c r="P171" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q171" s="30">
+        <v>0</v>
+      </c>
+      <c r="R171" s="30">
+        <v>0</v>
+      </c>
+      <c r="S171" s="30">
+        <v>0</v>
+      </c>
+      <c r="T171" s="30">
+        <v>0</v>
+      </c>
+      <c r="U171" s="30">
+        <v>0</v>
+      </c>
+      <c r="V171" s="30">
+        <v>0</v>
+      </c>
+      <c r="W171" s="30">
+        <v>0</v>
       </c>
       <c r="X171" s="21">
         <v>0</v>
       </c>
-      <c r="Y171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD171" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE171" s="21" t="s">
-        <v>14</v>
+      <c r="Y171" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z171" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA171" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB171" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC171" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD171" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE171" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:31" x14ac:dyDescent="0.35">
@@ -18036,7 +18051,7 @@
         <v>151</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="E172" s="19"/>
       <c r="F172" s="19"/>
@@ -18055,65 +18070,65 @@
       <c r="K172" s="21">
         <v>0</v>
       </c>
-      <c r="L172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="N172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="R172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="T172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="U172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="V172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="W172" s="21" t="s">
-        <v>14</v>
+      <c r="L172" s="30">
+        <v>0</v>
+      </c>
+      <c r="M172" s="30">
+        <v>0</v>
+      </c>
+      <c r="N172" s="30">
+        <v>0</v>
+      </c>
+      <c r="O172" s="30">
+        <v>0</v>
+      </c>
+      <c r="P172" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q172" s="30">
+        <v>0</v>
+      </c>
+      <c r="R172" s="30">
+        <v>0</v>
+      </c>
+      <c r="S172" s="30">
+        <v>0</v>
+      </c>
+      <c r="T172" s="30">
+        <v>0</v>
+      </c>
+      <c r="U172" s="30">
+        <v>0</v>
+      </c>
+      <c r="V172" s="30">
+        <v>0</v>
+      </c>
+      <c r="W172" s="30">
+        <v>0</v>
       </c>
       <c r="X172" s="21">
         <v>0</v>
       </c>
-      <c r="Y172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD172" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE172" s="21" t="s">
-        <v>14</v>
+      <c r="Y172" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z172" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA172" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB172" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC172" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD172" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE172" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>